<commit_message>
Project Proposal: Acceptance and Suggestions updated
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Proposal.xlsx
+++ b/project/MRU Java FSD Project Proposal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ByteXL\MRU\Java_FSD\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="130">
   <si>
     <t>Timestamp</t>
   </si>
@@ -400,6 +400,17 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Block Chain required.
+Alternative Idea id provided</t>
+  </si>
+  <si>
+    <t>No information regarding implementation</t>
+  </si>
+  <si>
+    <t>Developing a full-featured social media application may take longer than expected for third-year students.
+Alternative Idea is provided</t>
   </si>
 </sst>
 </file>
@@ -700,7 +711,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -743,6 +754,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -750,7 +767,67 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -901,9 +978,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Form responses 1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="secondRowStripe" dxfId="17"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -918,17 +995,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I29" headerRowDxfId="10" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I29" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="9">
-    <tableColumn id="1" name="Timestamp" dataDxfId="9"/>
-    <tableColumn id="2" name="University " dataDxfId="8"/>
-    <tableColumn id="3" name="Department" dataDxfId="7"/>
-    <tableColumn id="4" name="Project Title" dataDxfId="6"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="5"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="4"/>
-    <tableColumn id="7" name="Project Proposal" dataDxfId="3"/>
-    <tableColumn id="8" name="Status" dataDxfId="2"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="1"/>
+    <tableColumn id="1" name="Timestamp" dataDxfId="14"/>
+    <tableColumn id="2" name="University " dataDxfId="13"/>
+    <tableColumn id="3" name="Department" dataDxfId="12"/>
+    <tableColumn id="4" name="Project Title" dataDxfId="11"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="10"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="9"/>
+    <tableColumn id="7" name="Project Proposal" dataDxfId="8"/>
+    <tableColumn id="8" name="Status" dataDxfId="7"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Form responses 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1137,9 +1214,9 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1152,11 +1229,11 @@
     <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="66.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5546875" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="35.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1459,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>45680.751413449078</v>
       </c>
@@ -1405,9 +1482,11 @@
         <v>40</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I9" s="11"/>
+        <v>123</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
@@ -1432,11 +1511,13 @@
         <v>44</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>45680.77665782407</v>
       </c>
@@ -1459,9 +1540,11 @@
         <v>48</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" s="11"/>
+        <v>123</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
@@ -1950,6 +2033,17 @@
       <c r="I29" s="11"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Rejected">
+      <formula>NOT(ISERROR(SEARCH("Rejected",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Accepted">
+      <formula>NOT(ISERROR(SEARCH("Accepted",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>

</xml_diff>

<commit_message>
React_Basics: Layout example added, Project Proposal updated
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Proposal.xlsx
+++ b/project/MRU Java FSD Project Proposal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="238">
   <si>
     <t>Timestamp</t>
   </si>
@@ -291,16 +291,7 @@
     <t>https://drive.google.com/open?id=1mX62CI_ZnMWNQ8RIcN_epo_gbBRVxdqK</t>
   </si>
   <si>
-    <t>SHELF MASTER</t>
-  </si>
-  <si>
-    <t>P.Vamshi</t>
-  </si>
-  <si>
     <t>2211CS030137</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1CC4J_MLpC8RamXjpSQe_dU38f7_4PsQh</t>
   </si>
   <si>
     <t>Movie Review Application</t>
@@ -467,28 +458,10 @@
     <t>https://drive.google.com/open?id=1OAft75_NEewtAC1zCgrSUcmUMukZLa9o</t>
   </si>
   <si>
-    <t>HealthDock</t>
-  </si>
-  <si>
-    <t>V. Mamatha</t>
-  </si>
-  <si>
     <t>2211CS030168</t>
   </si>
   <si>
-    <t>https://drive.google.com/open?id=1wpn9pxfC-kOsbcWN5bUxWskFAfpETj7f</t>
-  </si>
-  <si>
-    <t>TALENTLINK</t>
-  </si>
-  <si>
     <t>M.Pravalika</t>
-  </si>
-  <si>
-    <t>2211CS030123</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1zBl-tb5lAuMA7rjJ64rTiKWvp5kOhUXf</t>
   </si>
   <si>
     <t>CHAT APPLICATION</t>
@@ -625,15 +598,6 @@
     <t>https://drive.google.com/open?id=18ijExkMBtC4OOUwPDEMnid1FPtV8wNsY</t>
   </si>
   <si>
-    <t>personal portfolio</t>
-  </si>
-  <si>
-    <t>Pravalika</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1PwZ9RmZu53oWZ-zgLZ5yGDjUYvHSCim9</t>
-  </si>
-  <si>
     <t>Abhishek Pandey</t>
   </si>
   <si>
@@ -664,13 +628,6 @@
     <t>Over Exhaused and Lack of Innovative ideas.</t>
   </si>
   <si>
-    <t>Over Exhaused and Lack of Innovative ideas.
-Stack is Java FSD not MERN stack.</t>
-  </si>
-  <si>
-    <t>Project Title taken with refined idea</t>
-  </si>
-  <si>
     <t>Limited Scope for Innovation and common use case.
 Duplicate Idea</t>
   </si>
@@ -731,10 +688,6 @@
     <t>Lack of innovative ideas</t>
   </si>
   <si>
-    <t>Lack of innovative ideas
-Duplicate idea</t>
-  </si>
-  <si>
     <t>find a way</t>
   </si>
   <si>
@@ -751,6 +704,45 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1x-xg5yzJXuJNHV6dcOrY6h1aAjD5F2MS</t>
+  </si>
+  <si>
+    <t>PG made EAZY</t>
+  </si>
+  <si>
+    <t>Vamshi</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1RisMErNOnXSzss2ZT6Z7xfxM5dsah6xf</t>
+  </si>
+  <si>
+    <t>FashionFiesta</t>
+  </si>
+  <si>
+    <t>pravalika</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1aWxLs2eAL6H1ok7baOo5rFApjaLkZ8HR</t>
+  </si>
+  <si>
+    <t>HerHaven</t>
+  </si>
+  <si>
+    <t>V.Mamatha</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1muKDiYMRcRuP9PQiH02x-Be2QFaqaR4y</t>
+  </si>
+  <si>
+    <t>QUICKWHEELZ</t>
+  </si>
+  <si>
+    <t>2211cs030123</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1UAsi-oto9nNxsYtLG1ApFI7iIQxt2bxu</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -916,7 +908,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1227,6 +1219,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1235,7 +1302,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1313,19 +1380,10 @@
     <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1359,6 +1417,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="17" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="17" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1368,7 +1444,127 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1494,96 +1690,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
@@ -1610,9 +1716,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Form responses 1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="firstRowStripe" dxfId="24"/>
+      <tableStyleElement type="secondRowStripe" dxfId="23"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1627,17 +1733,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I52" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I52" headerRowDxfId="22" dataDxfId="21">
   <tableColumns count="9">
-    <tableColumn id="1" name="Timestamp" dataDxfId="8"/>
-    <tableColumn id="2" name="University " dataDxfId="7"/>
-    <tableColumn id="3" name="Department" dataDxfId="6"/>
-    <tableColumn id="4" name="Project Title" dataDxfId="5"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="4"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="3"/>
-    <tableColumn id="7" name="Project Proposal" dataDxfId="2"/>
-    <tableColumn id="8" name="Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="0"/>
+    <tableColumn id="1" name="Timestamp" dataDxfId="20"/>
+    <tableColumn id="2" name="University " dataDxfId="19"/>
+    <tableColumn id="3" name="Department" dataDxfId="18"/>
+    <tableColumn id="4" name="Project Title" dataDxfId="17"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="16"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="15"/>
+    <tableColumn id="7" name="Project Proposal" dataDxfId="14"/>
+    <tableColumn id="8" name="Status" dataDxfId="13"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Form responses 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1847,7 +1953,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -1888,10 +1994,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.4">
@@ -1917,10 +2023,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.4">
@@ -1940,13 +2046,13 @@
         <v>14</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I3" s="14"/>
     </row>
@@ -1973,7 +2079,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I4" s="14"/>
     </row>
@@ -2000,10 +2106,10 @@
         <v>23</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.4">
@@ -2029,7 +2135,7 @@
         <v>27</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I6" s="14"/>
     </row>
@@ -2056,10 +2162,10 @@
         <v>31</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.4">
@@ -2085,10 +2191,10 @@
         <v>35</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8">
@@ -2108,16 +2214,16 @@
         <v>37</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="66.599999999999994">
@@ -2143,10 +2249,10 @@
         <v>43</v>
       </c>
       <c r="H10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.4">
@@ -2172,10 +2278,10 @@
         <v>47</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.4">
@@ -2201,10 +2307,10 @@
         <v>51</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.4">
@@ -2230,10 +2336,10 @@
         <v>55</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="43.2">
@@ -2259,10 +2365,10 @@
         <v>59</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="28.2">
@@ -2288,10 +2394,10 @@
         <v>63</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.4">
@@ -2317,10 +2423,10 @@
         <v>67</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.4">
@@ -2346,7 +2452,7 @@
         <v>71</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I17" s="14"/>
     </row>
@@ -2373,10 +2479,10 @@
         <v>77</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="43.2">
@@ -2402,10 +2508,10 @@
         <v>81</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.4">
@@ -2431,7 +2537,7 @@
         <v>85</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I20" s="14"/>
     </row>
@@ -2458,363 +2564,361 @@
         <v>89</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I21" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="53.4">
+      <c r="A22" s="19">
+        <v>45680.908493414347</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.4">
-      <c r="A22" s="16">
-        <v>45680.907292719909</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" s="27" t="s">
-        <v>193</v>
-      </c>
-    </row>
     <row r="23" spans="1:9" ht="53.4">
-      <c r="A23" s="19">
-        <v>45680.908493414347</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="20" t="s">
+      <c r="A23" s="16">
+        <v>45680.922215578699</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="G23" s="21" t="s">
+      <c r="F23" s="17" t="s">
         <v>96</v>
       </c>
+      <c r="G23" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="H23" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I23" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.4">
+      <c r="A24" s="19">
+        <v>45680.925850671294</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.4">
+      <c r="A25" s="16">
+        <v>45680.926538622683</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.4">
+      <c r="A26" s="19">
+        <v>45680.928315821759</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="42">
+      <c r="A27" s="16">
+        <v>45680.928983043981</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A28" s="19">
+        <v>45680.930342662032</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A29" s="16">
+        <v>45680.947892314813</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="17" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="53.4">
-      <c r="A24" s="16">
-        <v>45680.922215578699</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I24" s="15" t="s">
+      <c r="G29" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A30" s="19">
+        <v>45680.953972048606</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.4">
-      <c r="A25" s="19">
-        <v>45680.925850671294</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I25" s="14" t="s">
+      <c r="G30" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.4">
+      <c r="A31" s="16">
+        <v>45680.955453784722</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="17" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="14.4">
-      <c r="A26" s="16">
-        <v>45680.926538622683</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.4">
-      <c r="A27" s="19">
-        <v>45680.928315821759</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="21" t="s">
+      <c r="G31" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I27" s="27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="42">
-      <c r="A28" s="16">
-        <v>45680.928983043981</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="27" t="s">
+      <c r="I31" s="27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.4">
+      <c r="A32" s="19">
+        <v>45680.957277766203</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="19">
-        <v>45680.930342662032</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I29" s="27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="16">
-        <v>45680.947892314813</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I30" s="26" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A31" s="19">
-        <v>45680.953972048606</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I31" s="26" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.4">
-      <c r="A32" s="16">
-        <v>45680.955453784722</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="21" t="s">
         <v>135</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.4">
-      <c r="A33" s="19">
-        <v>45680.957277766203</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A33" s="16">
+        <v>45680.95775159722</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="G33" s="21" t="s">
+      <c r="F33" s="17" t="s">
         <v>138</v>
       </c>
+      <c r="G33" s="18" t="s">
+        <v>139</v>
+      </c>
       <c r="H33" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I33" s="27" t="s">
-        <v>210</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1">
       <c r="A34" s="16">
-        <v>45680.95775159722</v>
+        <v>45680.96231717593</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>7</v>
@@ -2823,226 +2927,228 @@
         <v>8</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I34" s="26"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A35" s="16">
-        <v>45680.96231717593</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="G35" s="18" t="s">
+    <row r="35" spans="1:9" ht="55.8">
+      <c r="A35" s="19">
+        <v>45680.986153298611</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>147</v>
       </c>
+      <c r="E35" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>150</v>
+      </c>
       <c r="H35" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I35" s="26"/>
-    </row>
-    <row r="36" spans="1:9" ht="55.8">
-      <c r="A36" s="19">
-        <v>45680.968409479166</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="G36" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="28.2">
+      <c r="A36" s="16">
+        <v>45680.991642835652</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="17" t="s">
         <v>151</v>
       </c>
+      <c r="E36" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>154</v>
+      </c>
       <c r="H36" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I36" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="55.8">
+      <c r="A37" s="19">
+        <v>45680.9927756713</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="28.2">
+      <c r="A38" s="16">
+        <v>45680.999614849541</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A39" s="19">
+        <v>45681.002351527779</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="28.2">
+      <c r="A40" s="19">
+        <v>45681.437269351853</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A41" s="16">
+        <v>45681.455018865745</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="17" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A37" s="16">
-        <v>45680.981185868055</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I37" s="27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="55.8">
-      <c r="A38" s="19">
-        <v>45680.986153298611</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I38" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="28.2">
-      <c r="A39" s="16">
-        <v>45680.991642835652</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I39" s="27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="55.8">
-      <c r="A40" s="19">
-        <v>45680.9927756713</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="G40" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I40" s="27" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="28.2">
-      <c r="A41" s="16">
-        <v>45680.999614849541</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>173</v>
-      </c>
       <c r="G41" s="18" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I41" s="27" t="s">
-        <v>211</v>
+        <v>114</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1">
       <c r="A42" s="19">
-        <v>45681.002351527779</v>
+        <v>45681.476912754631</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>7</v>
@@ -3051,339 +3157,335 @@
         <v>8</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F42" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I42" s="27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A43" s="16">
+        <v>45681.542123009262</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I43" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A44" s="22">
+        <v>45681.868537847222</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I44" s="27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="42">
+      <c r="A45" s="28">
+        <v>45681.990429247686</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I45" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A46" s="31">
+        <v>45682.458358969903</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="G46" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I46" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A47" s="34">
+        <v>45684.390717592592</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="I47" s="14"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A48" s="38">
+        <v>45684.543680555558</v>
+      </c>
+      <c r="B48" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="F48" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="H48" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="I48" s="42"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A49" s="34">
+        <v>45685.31763888889</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="G42" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I42" s="26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="28.2">
-      <c r="A43" s="19">
-        <v>45681.437269351853</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I43" s="27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A44" s="16">
-        <v>45681.455018865745</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="F44" s="17" t="s">
+      <c r="E49" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="G44" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I44" s="26" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A45" s="19">
-        <v>45681.476912754631</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F45" s="20" t="s">
+      <c r="F49" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G49" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="G45" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I45" s="27" t="s">
+      <c r="H49" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="I49" s="14"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A50" s="43">
+        <v>45685.793958333335</v>
+      </c>
+      <c r="B50" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="E50" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="F50" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="G50" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A46" s="16">
-        <v>45681.542123009262</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I46" s="27" t="s">
+      <c r="H50" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A51" s="44">
+        <v>45685.897152777776</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="46" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A47" s="22">
-        <v>45681.868537847222</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F47" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="G47" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I47" s="27" t="s">
+      <c r="E51" s="46" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="42">
-      <c r="A48" s="28">
-        <v>45681.990429247686</v>
-      </c>
-      <c r="B48" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="30" t="s">
+      <c r="F51" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="G51" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="H51" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="I51" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="E48" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="F48" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="G48" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I48" s="27" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="42">
-      <c r="A49" s="29">
-        <v>45682.392727604165</v>
-      </c>
-      <c r="B49" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="F49" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="G49" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I49" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A50" s="34">
-        <v>45682.458358969903</v>
-      </c>
-      <c r="B50" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="E50" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="F50" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="G50" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I50" s="27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A51" s="37">
-        <v>45684.390717592592</v>
-      </c>
-      <c r="B51" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="38" t="s">
+    </row>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A52" s="38">
+        <v>45685.91777777778</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="E51" s="38" t="s">
+      <c r="E52" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="F52" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="F51" s="38" t="s">
+      <c r="G52" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="G51" s="39" t="s">
+      <c r="H52" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="H51" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="I51" s="14"/>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A52" s="41">
-        <v>45684.543680555558</v>
-      </c>
-      <c r="B52" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="F52" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="G52" s="43" t="s">
-        <v>239</v>
-      </c>
-      <c r="H52" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="I52" s="45"/>
+      <c r="I52" s="42"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H51:H1048576 H1:H49">
-    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="Pending">
+  <conditionalFormatting sqref="H47:H1048576 H1:H45">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",H50)))</formula>
+  <conditionalFormatting sqref="H46">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Accepted">
-      <formula>NOT(ISERROR(SEARCH("Accepted",H50)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Accepted">
+      <formula>NOT(ISERROR(SEARCH("Accepted",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Rejected">
-      <formula>NOT(ISERROR(SEARCH("Rejected",H50)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Rejected">
+      <formula>NOT(ISERROR(SEARCH("Rejected",H46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F52">
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="69"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>

</xml_diff>

<commit_message>
JavaScript: call-back and arrow fn example is added. React: state example is added.
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Proposal.xlsx
+++ b/project/MRU Java FSD Project Proposal.xlsx
@@ -1052,19 +1052,65 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1094,31 +1140,10 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
@@ -1133,14 +1158,11 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1259,20 +1281,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1378,36 +1386,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
@@ -1434,9 +1412,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Form responses 1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="firstRowStripe" dxfId="24"/>
-      <tableStyleElement type="secondRowStripe" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="secondRowStripe" dxfId="21"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1451,17 +1429,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I55" headerRowDxfId="10" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I55" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I55"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Timestamp" dataDxfId="9"/>
     <tableColumn id="2" name="University " dataDxfId="8"/>
     <tableColumn id="3" name="Department" dataDxfId="7"/>
     <tableColumn id="4" name="Project Title" dataDxfId="6"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="2"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="7" name="Project Proposal" dataDxfId="1"/>
-    <tableColumn id="8" name="Status" dataDxfId="5"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="4"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="5"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="Project Proposal" dataDxfId="3"/>
+    <tableColumn id="8" name="Status" dataDxfId="2"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1670,9 +1649,9 @@
   </sheetPr>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3262,33 +3241,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H46:H1048576 H1:H44">
-    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",H45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",H45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",H45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F55">
-    <cfRule type="duplicateValues" dxfId="11" priority="98"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="98"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>

</xml_diff>

<commit_message>
React Basics: conditional rendering and useEffect updated
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Proposal.xlsx
+++ b/project/MRU Java FSD Project Proposal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="252">
   <si>
     <t>Timestamp</t>
   </si>
@@ -353,18 +353,6 @@
 Alternative Idea is provided</t>
   </si>
   <si>
-    <t>Library Management System</t>
-  </si>
-  <si>
-    <t>Sita Leela Manas Jagannath</t>
-  </si>
-  <si>
-    <t>2211CS030152</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=14UntdKgoEMp1Rn2YyfAHFkJbNKMRjVqL</t>
-  </si>
-  <si>
     <t>Asinshaik</t>
   </si>
   <si>
@@ -544,10 +532,6 @@
   </si>
   <si>
     <t>Idea is refined.</t>
-  </si>
-  <si>
-    <t>Lack of Innovative ideas.
-Duplicate ideas.</t>
   </si>
   <si>
     <t>Over Exhaused and Lack of Innovative ideas.</t>
@@ -1072,312 +1056,114 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="34">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF006100"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF9C6500"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
+        <color rgb="FF006100"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C6500"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1470,6 +1256,312 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
@@ -1496,9 +1588,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Form responses 1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1513,18 +1605,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I58" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:I57" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:I57"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Timestamp" dataDxfId="8"/>
-    <tableColumn id="2" name="University " dataDxfId="7"/>
-    <tableColumn id="3" name="Department" dataDxfId="6"/>
-    <tableColumn id="4" name="Project Title" dataDxfId="5"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="4"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="7" name="Project Proposal" dataDxfId="2"/>
-    <tableColumn id="8" name="Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="0"/>
+    <tableColumn id="1" name="Timestamp" dataDxfId="28"/>
+    <tableColumn id="2" name="University " dataDxfId="27"/>
+    <tableColumn id="3" name="Department" dataDxfId="26"/>
+    <tableColumn id="4" name="Project Title" dataDxfId="25"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="24"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="Project Proposal" dataDxfId="22"/>
+    <tableColumn id="8" name="Status" dataDxfId="21"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1731,11 +1823,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="A2:I58"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1827,7 +1919,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>15</v>
@@ -1995,7 +2087,7 @@
         <v>37</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>38</v>
@@ -2120,7 +2212,7 @@
         <v>105</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
@@ -2149,7 +2241,7 @@
         <v>105</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2178,7 +2270,7 @@
         <v>105</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2234,7 +2326,7 @@
         <v>105</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2290,7 +2382,7 @@
         <v>105</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2310,7 +2402,7 @@
         <v>85</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>86</v>
@@ -2319,7 +2411,7 @@
         <v>105</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2348,7 +2440,7 @@
         <v>105</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2377,7 +2469,7 @@
         <v>107</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2435,12 +2527,12 @@
         <v>105</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
-        <v>45680.928983043981</v>
+        <v>45680.947892314813</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>7</v>
@@ -2449,27 +2541,27 @@
         <v>8</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>113</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>173</v>
+        <v>107</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
-        <v>45680.947892314813</v>
+        <v>45680.953972048606</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>7</v>
@@ -2478,27 +2570,27 @@
         <v>8</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="F26" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>107</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
-        <v>45680.953972048606</v>
+        <v>45680.955453784722</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>7</v>
@@ -2507,27 +2599,27 @@
         <v>8</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="F27" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>120</v>
-      </c>
       <c r="H27" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>172</v>
+        <v>105</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
-        <v>45680.955453784722</v>
+        <v>45680.95775159722</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>7</v>
@@ -2536,27 +2628,25 @@
         <v>8</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="F28" s="23" t="s">
         <v>122</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>182</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>123</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>163</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
-        <v>45680.95775159722</v>
+        <v>45680.96231717593</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>7</v>
@@ -2565,25 +2655,25 @@
         <v>8</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>107</v>
       </c>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
-        <v>45680.96231717593</v>
+        <v>45680.991642835652</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>7</v>
@@ -2592,25 +2682,27 @@
         <v>8</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
-        <v>45680.991642835652</v>
+        <v>45680.9927756713</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>7</v>
@@ -2625,21 +2717,21 @@
         <v>136</v>
       </c>
       <c r="F31" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>105</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
-        <v>45680.9927756713</v>
+        <v>45680.999614849541</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>7</v>
@@ -2648,27 +2740,27 @@
         <v>8</v>
       </c>
       <c r="D32" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="F32" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>105</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
-        <v>45680.999614849541</v>
+        <v>45681.437269351853</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>7</v>
@@ -2683,21 +2775,21 @@
         <v>143</v>
       </c>
       <c r="F33" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>105</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
-        <v>45681.437269351853</v>
+        <v>45681.455018865745</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>7</v>
@@ -2712,21 +2804,21 @@
         <v>147</v>
       </c>
       <c r="F34" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>149</v>
-      </c>
       <c r="H34" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>174</v>
+        <v>107</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
-        <v>45681.455018865745</v>
+        <v>45681.542123009262</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>7</v>
@@ -2741,21 +2833,21 @@
         <v>151</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>152</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>172</v>
+        <v>105</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
-        <v>45681.542123009262</v>
+        <v>45681.868537847222</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>7</v>
@@ -2764,13 +2856,13 @@
         <v>8</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="F36" s="23" t="s">
         <v>155</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>185</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>156</v>
@@ -2779,12 +2871,12 @@
         <v>105</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
-        <v>45681.868537847222</v>
+        <v>45682.458358969903</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>7</v>
@@ -2793,74 +2885,72 @@
         <v>8</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>105</v>
       </c>
       <c r="I37" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="15">
+        <v>45684.390717592592</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="19">
+        <v>45684.543680555558</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
-        <v>45682.458358969903</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15">
-        <v>45684.390717592592</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="16" t="s">
+      <c r="F39" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="21" t="s">
         <v>188</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="H39" s="18" t="s">
         <v>107</v>
@@ -2868,26 +2958,26 @@
       <c r="I39" s="11"/>
     </row>
     <row r="40" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19">
-        <v>45684.543680555558</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>192</v>
+      <c r="A40" s="15">
+        <v>45685.31763888889</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>190</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G40" s="21" t="s">
-        <v>193</v>
+        <v>83</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>191</v>
       </c>
       <c r="H40" s="18" t="s">
         <v>107</v>
@@ -2896,7 +2986,7 @@
     </row>
     <row r="41" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
-        <v>45685.31763888889</v>
+        <v>45685.897152777776</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>7</v>
@@ -2905,72 +2995,74 @@
         <v>8</v>
       </c>
       <c r="D41" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E41" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="F41" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" s="17" t="s">
         <v>195</v>
-      </c>
-      <c r="F41" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>196</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="I41" s="11"/>
+      <c r="I41" s="11" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="42" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="15">
-        <v>45685.897152777776</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="16" t="s">
+      <c r="A42" s="19">
+        <v>45685.91777777778</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="G42" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="H42" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="15">
+        <v>45686.616516203707</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F42" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="G42" s="17" t="s">
+      <c r="E43" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="H42" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19">
-        <v>45685.91777777778</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="20" t="s">
+      <c r="F43" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="E43" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="F43" s="23" t="s">
+      <c r="G43" s="17" t="s">
         <v>202</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>203</v>
       </c>
       <c r="H43" s="18" t="s">
         <v>105</v>
@@ -2979,38 +3071,38 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="15">
-        <v>45686.616516203707</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="16" t="s">
+    <row r="44" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="19">
+        <v>45686.64234953704</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="F44" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="F44" s="23" t="s">
+      <c r="G44" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G44" s="17" t="s">
-        <v>207</v>
-      </c>
       <c r="H44" s="18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
-        <v>45686.64234953704</v>
+        <v>45686.841932870368</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>7</v>
@@ -3024,67 +3116,65 @@
       <c r="E45" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="F45" s="23">
+        <v>109</v>
+      </c>
+      <c r="G45" s="21" t="s">
         <v>210</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>211</v>
       </c>
       <c r="H45" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="I45" s="11" t="s">
-        <v>219</v>
-      </c>
+      <c r="I45" s="11"/>
     </row>
     <row r="46" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19">
-        <v>45686.841932870368</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="20" t="s">
+      <c r="A46" s="15">
+        <v>45686.932685185187</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="G46" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="F46" s="23">
-        <v>109</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>215</v>
       </c>
       <c r="H46" s="18" t="s">
         <v>107</v>
       </c>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="15">
-        <v>45686.932685185187</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="16" t="s">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19">
+        <v>45686.964131944442</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="E47" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F47" s="23" t="s">
+      <c r="G47" s="21" t="s">
         <v>217</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>218</v>
       </c>
       <c r="H47" s="18" t="s">
         <v>107</v>
@@ -3092,26 +3182,26 @@
       <c r="I47" s="11"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="19">
-        <v>45686.964131944442</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="20" t="s">
+      <c r="A48" s="15">
+        <v>45687.545451388891</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="17" t="s">
         <v>220</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="G48" s="21" t="s">
-        <v>222</v>
       </c>
       <c r="H48" s="18" t="s">
         <v>107</v>
@@ -3119,82 +3209,82 @@
       <c r="I48" s="11"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="15">
-        <v>45687.545451388891</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="16" t="s">
+      <c r="A49" s="19">
+        <v>45687.759386574071</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15">
+        <v>45687.795474537037</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E50" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="F49" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G49" s="17" t="s">
+      <c r="F50" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="H49" s="18" t="s">
+      <c r="G50" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="H50" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="I49" s="11"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="19">
-        <v>45687.759386574071</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="E50" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F50" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="G50" s="21" t="s">
+      <c r="I50" s="11"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="19">
+        <v>45687.801678240743</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="H50" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15">
-        <v>45687.795474537037</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="16" t="s">
+      <c r="E51" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="F51" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="G51" s="21" t="s">
         <v>229</v>
-      </c>
-      <c r="F51" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>231</v>
       </c>
       <c r="H51" s="18" t="s">
         <v>107</v>
@@ -3202,26 +3292,26 @@
       <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19">
-        <v>45687.801678240743</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="20" t="s">
+      <c r="A52" s="15">
+        <v>45687.829421296294</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="F52" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="E52" s="20" t="s">
+      <c r="G52" s="17" t="s">
         <v>233</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="G52" s="21" t="s">
-        <v>234</v>
       </c>
       <c r="H52" s="18" t="s">
         <v>107</v>
@@ -3229,82 +3319,82 @@
       <c r="I52" s="11"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="15">
-        <v>45687.829421296294</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="16" t="s">
+      <c r="A53" s="19">
+        <v>45687.990185185183</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="E53" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="F53" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="F53" s="24" t="s">
+      <c r="G53" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="H53" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15">
+        <v>45688.00571759259</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="E54" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="H54" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="I53" s="11"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="19">
-        <v>45687.990185185183</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="F54" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="G54" s="21" t="s">
+      <c r="I54" s="11"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="19">
+        <v>45688.477754629632</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="H54" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="15">
-        <v>45688.00571759259</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="16" t="s">
+      <c r="E55" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="F55" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="G55" s="21" t="s">
         <v>244</v>
-      </c>
-      <c r="F55" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>246</v>
       </c>
       <c r="H55" s="18" t="s">
         <v>107</v>
@@ -3312,26 +3402,26 @@
       <c r="I55" s="11"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="19">
-        <v>45688.477754629632</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="20" t="s">
+      <c r="A56" s="15">
+        <v>45688.909166666665</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G56" s="17" t="s">
         <v>247</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="G56" s="21" t="s">
-        <v>249</v>
       </c>
       <c r="H56" s="18" t="s">
         <v>107</v>
@@ -3339,88 +3429,62 @@
       <c r="I56" s="11"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="15">
-        <v>45688.909166666665</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="16" t="s">
+      <c r="A57" s="19">
+        <v>45688.980833333335</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="F57" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="G57" s="21" t="s">
         <v>251</v>
-      </c>
-      <c r="F57" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="G57" s="17" t="s">
-        <v>252</v>
       </c>
       <c r="H57" s="18" t="s">
         <v>107</v>
       </c>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="19">
-        <v>45688.980833333335</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="F58" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="G58" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="I58" s="11"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="H39:H1048576 H1:H37">
-    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="Pending">
+  <conditionalFormatting sqref="H38:H1048576 H1:H36">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",H38)))</formula>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",H37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Accepted">
-      <formula>NOT(ISERROR(SEARCH("Accepted",H38)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Accepted">
+      <formula>NOT(ISERROR(SEARCH("Accepted",H37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Rejected">
-      <formula>NOT(ISERROR(SEARCH("Rejected",H38)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Rejected">
+      <formula>NOT(ISERROR(SEARCH("Rejected",H37)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F58">
-    <cfRule type="duplicateValues" dxfId="11" priority="199"/>
+  <conditionalFormatting sqref="F1:F57">
+    <cfRule type="duplicateValues" dxfId="1" priority="216"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
@@ -3479,12 +3543,11 @@
     <hyperlink ref="G55" r:id="rId54"/>
     <hyperlink ref="G56" r:id="rId55"/>
     <hyperlink ref="G57" r:id="rId56"/>
-    <hyperlink ref="G58" r:id="rId57"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
   <tableParts count="1">
-    <tablePart r:id="rId59"/>
+    <tablePart r:id="rId58"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>